<commit_message>
Inserção e testes com fáculas
</commit_message>
<xml_diff>
--- a/Exoplanets/GJ9827d/Parâmetros.xlsx
+++ b/Exoplanets/GJ9827d/Parâmetros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\GJ9827d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A156AE-3DCB-462B-9081-6459335686C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07B4BF7-0A80-457A-8FE9-F6B8D28A8043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13545" yWindow="1845" windowWidth="19155" windowHeight="13575" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
+    <workbookView xWindow="19245" yWindow="2025" windowWidth="19155" windowHeight="13575" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -763,7 +763,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="18">
         <v>0.1</v>

</xml_diff>